<commit_message>
Added ident layer to gerbers and finalised Pick and Place data
</commit_message>
<xml_diff>
--- a/schematics/Full Board Prototype/BOM - Pick & Place etc/Pick & Place.xlsx
+++ b/schematics/Full Board Prototype/BOM - Pick & Place etc/Pick & Place.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="161">
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>CLOCK</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Value/Part</t>
   </si>
 </sst>
 </file>
@@ -1364,8 +1364,8 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J83" sqref="J83"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,45 +1379,45 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="5">
         <v>1432109</v>
@@ -1432,21 +1432,21 @@
         <v>270</v>
       </c>
       <c r="I2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="5">
         <v>1432109</v>
@@ -1461,21 +1461,21 @@
         <v>270</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="5">
         <v>1432109</v>
@@ -1490,21 +1490,21 @@
         <v>270</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5" s="5">
         <v>1572631</v>
@@ -1519,21 +1519,21 @@
         <v>270</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="5">
         <v>1572631</v>
@@ -1548,21 +1548,21 @@
         <v>270</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="5">
         <v>1572631</v>
@@ -1577,21 +1577,21 @@
         <v>270</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="5">
         <v>1907038</v>
@@ -1606,21 +1606,21 @@
         <v>90</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" s="5">
         <v>1907038</v>
@@ -1635,21 +1635,21 @@
         <v>90</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" s="5">
         <v>1907038</v>
@@ -1664,21 +1664,21 @@
         <v>90</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="6">
         <v>2320760</v>
@@ -1693,21 +1693,21 @@
         <v>0</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" s="6">
         <v>1758924</v>
@@ -1722,21 +1722,21 @@
         <v>180</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E13" s="6">
         <v>1758924</v>
@@ -1751,21 +1751,21 @@
         <v>0</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" s="6">
         <v>2320760</v>
@@ -1780,21 +1780,21 @@
         <v>180</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E15" s="6">
         <v>2320760</v>
@@ -1809,21 +1809,21 @@
         <v>0</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="6">
         <v>1758924</v>
@@ -1838,21 +1838,21 @@
         <v>180</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E17" s="6">
         <v>2320760</v>
@@ -1867,21 +1867,21 @@
         <v>270</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="5">
         <v>1135269</v>
@@ -1896,21 +1896,21 @@
         <v>270</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E19" s="5">
         <v>1135269</v>
@@ -1925,21 +1925,21 @@
         <v>270</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E20" s="6">
         <v>2320760</v>
@@ -1954,21 +1954,21 @@
         <v>270</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E21" s="5">
         <v>1135269</v>
@@ -1983,21 +1983,21 @@
         <v>270</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E22" s="6">
         <v>2320760</v>
@@ -2012,21 +2012,21 @@
         <v>270</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" s="6">
         <v>2320829</v>
@@ -2041,21 +2041,21 @@
         <v>0</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E24" s="6">
         <v>2320829</v>
@@ -2070,21 +2070,21 @@
         <v>0</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E25" s="6">
         <v>2320829</v>
@@ -2099,21 +2099,21 @@
         <v>0</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26" s="6">
         <v>2320776</v>
@@ -2128,21 +2128,21 @@
         <v>270</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E27" s="6">
         <v>2320776</v>
@@ -2157,21 +2157,21 @@
         <v>270</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E28" s="6">
         <v>2320776</v>
@@ -2186,21 +2186,21 @@
         <v>270</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E29" s="6">
         <v>2320760</v>
@@ -2215,21 +2215,21 @@
         <v>0</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E30" s="6">
         <v>2320760</v>
@@ -2244,21 +2244,21 @@
         <v>0</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E31" s="6">
         <v>2320760</v>
@@ -2273,21 +2273,21 @@
         <v>0</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E32" s="6">
         <v>2320776</v>
@@ -2302,21 +2302,21 @@
         <v>270</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E33" s="6">
         <v>2320776</v>
@@ -2331,21 +2331,21 @@
         <v>270</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E34" s="6">
         <v>2320776</v>
@@ -2360,21 +2360,21 @@
         <v>270</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E35" s="6">
         <v>2320760</v>
@@ -2389,21 +2389,21 @@
         <v>180</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E36" s="6">
         <v>2320760</v>
@@ -2418,21 +2418,21 @@
         <v>180</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E37" s="6">
         <v>2320760</v>
@@ -2447,21 +2447,21 @@
         <v>180</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
         <v>50</v>
       </c>
-      <c r="B38" t="s">
-        <v>51</v>
-      </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E38" s="5">
         <v>2362109</v>
@@ -2476,21 +2476,21 @@
         <v>270</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E39" s="5">
         <v>1288204</v>
@@ -2505,21 +2505,21 @@
         <v>90</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E40" s="5">
         <v>2362109</v>
@@ -2534,21 +2534,21 @@
         <v>270</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E41" s="5">
         <v>1288204</v>
@@ -2563,21 +2563,21 @@
         <v>90</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E42" s="5">
         <v>2362109</v>
@@ -2592,21 +2592,21 @@
         <v>270</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E43" s="5">
         <v>1288204</v>
@@ -2621,21 +2621,21 @@
         <v>90</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
         <v>57</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>58</v>
       </c>
-      <c r="C44" t="s">
-        <v>59</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E44" s="7">
         <v>1581966</v>
@@ -2650,21 +2650,21 @@
         <v>90</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
         <v>58</v>
       </c>
-      <c r="C45" t="s">
-        <v>59</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="7">
         <v>1581966</v>
@@ -2679,21 +2679,21 @@
         <v>90</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
         <v>58</v>
       </c>
-      <c r="C46" t="s">
-        <v>59</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E46" s="7">
         <v>1581966</v>
@@ -2708,21 +2708,21 @@
         <v>90</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
         <v>62</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>63</v>
       </c>
-      <c r="C47" t="s">
-        <v>64</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E47" s="5">
         <v>2067770</v>
@@ -2737,21 +2737,21 @@
         <v>0</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
         <v>63</v>
       </c>
-      <c r="C48" t="s">
-        <v>64</v>
-      </c>
       <c r="D48" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E48" s="5">
         <v>2067770</v>
@@ -2766,21 +2766,21 @@
         <v>0</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" t="s">
         <v>63</v>
       </c>
-      <c r="C49" t="s">
-        <v>64</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E49" s="5">
         <v>2067770</v>
@@ -2795,995 +2795,995 @@
         <v>0</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" t="s">
         <v>67</v>
       </c>
-      <c r="B50" t="s">
-        <v>68</v>
-      </c>
       <c r="C50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E50" s="7">
         <v>9732241</v>
       </c>
       <c r="F50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E51" s="7">
         <v>9732241</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E52" s="7">
         <v>9732241</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
         <v>71</v>
       </c>
-      <c r="C53" t="s">
-        <v>72</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E53" s="5">
         <v>1098038</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E54" s="5">
         <v>1098038</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E55" s="5">
         <v>1098038</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E56" s="5">
         <v>1098038</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G56" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E57" s="5">
         <v>1098038</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E58" s="5">
         <v>1098038</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E59" s="5">
         <v>1098038</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E60" s="5">
         <v>1098038</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E61" s="5">
         <v>1098038</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I61" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E62" s="5">
         <v>1098038</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I62" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E63" s="5">
         <v>1098038</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I63" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E64" s="5">
         <v>1098038</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I64" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E65" s="5">
         <v>1098038</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I65" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E66" s="5">
         <v>1098038</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I66" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E67" s="5">
         <v>1098038</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E68" s="5">
         <v>1098038</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E69" s="5">
         <v>1098038</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E70" s="5">
         <v>1098038</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G70" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E71" s="5">
         <v>1098038</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G71" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E72" s="5">
         <v>1098038</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E73" s="5">
         <v>1098038</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E74" s="5">
         <v>1098038</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E75" s="5">
         <v>1098038</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E76" s="5">
         <v>1098038</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E77" s="5">
         <v>1098038</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E78" s="5">
         <v>1098038</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E79" s="5">
         <v>1098038</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I79" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E80" s="5">
         <v>1098038</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I80" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E81" s="5">
         <v>1098038</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H81" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I81" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C82" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E82" s="5">
         <v>1098038</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G82" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I82" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C83" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E83" s="5">
         <v>1098038</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I83" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C84" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E84" s="5">
         <v>1098038</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G84" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" t="s">
         <v>104</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>105</v>
       </c>
-      <c r="C85" t="s">
-        <v>106</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E85" s="7">
         <v>9732241</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G85" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H85" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E86" s="7">
         <v>9732241</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G86" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I86" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" t="s">
         <v>108</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>109</v>
       </c>
-      <c r="C87" t="s">
-        <v>110</v>
-      </c>
       <c r="D87" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E87" s="7">
         <v>1468890</v>
@@ -3798,21 +3798,21 @@
         <v>180</v>
       </c>
       <c r="I87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B88" t="s">
+        <v>108</v>
+      </c>
+      <c r="C88" t="s">
         <v>109</v>
       </c>
-      <c r="C88" t="s">
-        <v>110</v>
-      </c>
       <c r="D88" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E88" s="7">
         <v>1468890</v>
@@ -3827,21 +3827,21 @@
         <v>180</v>
       </c>
       <c r="I88" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B89" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" t="s">
         <v>109</v>
       </c>
-      <c r="C89" t="s">
-        <v>110</v>
-      </c>
       <c r="D89" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E89" s="7">
         <v>1468890</v>
@@ -3856,21 +3856,21 @@
         <v>180</v>
       </c>
       <c r="I89" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>112</v>
+      </c>
+      <c r="B90" t="s">
         <v>113</v>
       </c>
-      <c r="B90" t="s">
-        <v>114</v>
-      </c>
       <c r="C90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E90" s="7">
         <v>2325323</v>
@@ -3885,21 +3885,21 @@
         <v>90</v>
       </c>
       <c r="I90" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E91" s="7">
         <v>2325323</v>
@@ -3914,21 +3914,21 @@
         <v>90</v>
       </c>
       <c r="I91" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E92" s="7">
         <v>2325323</v>
@@ -3943,21 +3943,21 @@
         <v>90</v>
       </c>
       <c r="I92" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" t="s">
         <v>117</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>118</v>
       </c>
-      <c r="C93" t="s">
-        <v>119</v>
-      </c>
       <c r="D93" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E93" s="6">
         <v>1838112</v>
@@ -3972,21 +3972,21 @@
         <v>180</v>
       </c>
       <c r="I93" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>119</v>
+      </c>
+      <c r="B94" t="s">
         <v>120</v>
       </c>
-      <c r="B94" t="s">
-        <v>121</v>
-      </c>
       <c r="C94" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E94" s="6">
         <v>1837879</v>
@@ -4001,21 +4001,21 @@
         <v>270</v>
       </c>
       <c r="I94" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C95" t="s">
         <v>118</v>
       </c>
-      <c r="C95" t="s">
-        <v>119</v>
-      </c>
       <c r="D95" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E95" s="6">
         <v>1838112</v>
@@ -4030,21 +4030,21 @@
         <v>180</v>
       </c>
       <c r="I95" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B96" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C96" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E96" s="6">
         <v>1837879</v>
@@ -4059,21 +4059,21 @@
         <v>270</v>
       </c>
       <c r="I96" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B97" t="s">
+        <v>117</v>
+      </c>
+      <c r="C97" t="s">
         <v>118</v>
       </c>
-      <c r="C97" t="s">
-        <v>119</v>
-      </c>
       <c r="D97" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E97" s="6">
         <v>1838112</v>
@@ -4088,21 +4088,21 @@
         <v>180</v>
       </c>
       <c r="I97" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B98" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C98" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E98" s="6">
         <v>1837879</v>
@@ -4117,21 +4117,21 @@
         <v>270</v>
       </c>
       <c r="I98" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>125</v>
+      </c>
+      <c r="B99" t="s">
         <v>126</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>127</v>
       </c>
-      <c r="C99" t="s">
-        <v>128</v>
-      </c>
       <c r="D99" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E99" s="6">
         <v>2131042</v>
@@ -4146,21 +4146,21 @@
         <v>270</v>
       </c>
       <c r="I99" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B100" t="s">
+        <v>126</v>
+      </c>
+      <c r="C100" t="s">
         <v>127</v>
       </c>
-      <c r="C100" t="s">
-        <v>128</v>
-      </c>
       <c r="D100" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E100" s="6">
         <v>2131042</v>
@@ -4175,21 +4175,21 @@
         <v>270</v>
       </c>
       <c r="I100" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B101" t="s">
+        <v>126</v>
+      </c>
+      <c r="C101" t="s">
         <v>127</v>
       </c>
-      <c r="C101" t="s">
-        <v>128</v>
-      </c>
       <c r="D101" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E101" s="6">
         <v>2131042</v>
@@ -4204,21 +4204,21 @@
         <v>270</v>
       </c>
       <c r="I101" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" t="s">
         <v>131</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>132</v>
       </c>
-      <c r="C102" t="s">
-        <v>133</v>
-      </c>
       <c r="D102" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E102" s="7">
         <v>2068091</v>
@@ -4233,21 +4233,21 @@
         <v>270</v>
       </c>
       <c r="I102" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B103" t="s">
+        <v>131</v>
+      </c>
+      <c r="C103" t="s">
         <v>132</v>
       </c>
-      <c r="C103" t="s">
-        <v>133</v>
-      </c>
       <c r="D103" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E103" s="7">
         <v>2068091</v>
@@ -4262,21 +4262,21 @@
         <v>270</v>
       </c>
       <c r="I103" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B104" t="s">
+        <v>131</v>
+      </c>
+      <c r="C104" t="s">
         <v>132</v>
       </c>
-      <c r="C104" t="s">
-        <v>133</v>
-      </c>
       <c r="D104" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E104" s="7">
         <v>2068091</v>
@@ -4291,21 +4291,21 @@
         <v>270</v>
       </c>
       <c r="I104" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>135</v>
+      </c>
+      <c r="B105" t="s">
         <v>136</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>137</v>
       </c>
-      <c r="C105" t="s">
-        <v>138</v>
-      </c>
       <c r="D105" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E105" s="7">
         <v>9604367</v>
@@ -4320,94 +4320,94 @@
         <v>0</v>
       </c>
       <c r="I105" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>138</v>
+      </c>
+      <c r="B106" t="s">
         <v>139</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>140</v>
       </c>
-      <c r="C106" t="s">
-        <v>141</v>
-      </c>
       <c r="D106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E106" s="6">
         <v>8391289</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H106" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I106" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>141</v>
+      </c>
+      <c r="B107" t="s">
         <v>142</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>143</v>
       </c>
-      <c r="C107" t="s">
-        <v>144</v>
-      </c>
       <c r="D107" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E107" s="6">
         <v>2294307</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H107" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I107" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>144</v>
+      </c>
+      <c r="B108" t="s">
         <v>145</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>146</v>
       </c>
-      <c r="C108" t="s">
-        <v>147</v>
-      </c>
       <c r="D108" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E108" s="6">
         <v>1084697</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H108" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I108" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Pick & Place Data and Ident Gerber File for PCB assembly
</commit_message>
<xml_diff>
--- a/schematics/Full Board Prototype/BOM - Pick & Place etc/Pick & Place.xlsx
+++ b/schematics/Full Board Prototype/BOM - Pick & Place etc/Pick & Place.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="161">
   <si>
     <t>CLOCK</t>
   </si>
@@ -1364,8 +1364,8 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3870,22 +3870,22 @@
         <v>113</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E90" s="7">
         <v>2325323</v>
       </c>
-      <c r="F90" s="12">
-        <v>42.86</v>
-      </c>
-      <c r="G90" s="12">
-        <v>102.68</v>
-      </c>
-      <c r="H90" s="12">
-        <v>90</v>
+      <c r="F90" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H90" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="I90" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3899,22 +3899,22 @@
         <v>113</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E91" s="7">
         <v>2325323</v>
       </c>
-      <c r="F91" s="12">
-        <v>42.86</v>
-      </c>
-      <c r="G91" s="12">
-        <v>66.17</v>
-      </c>
-      <c r="H91" s="12">
-        <v>90</v>
+      <c r="F91" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H91" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="I91" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3928,22 +3928,22 @@
         <v>113</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E92" s="7">
         <v>2325323</v>
       </c>
-      <c r="F92" s="12">
-        <v>42.86</v>
-      </c>
-      <c r="G92" s="12">
-        <v>31.24</v>
-      </c>
-      <c r="H92" s="12">
-        <v>90</v>
+      <c r="F92" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H92" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="I92" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4448,6 +4448,6 @@
     <hyperlink ref="E70:E84" r:id="rId25" tooltip="1098038" display="http://uk.farnell.com/fci/76341-308lf/socket-1row-8way/dp/1098038"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="landscape" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating Arduino code to program new switch board
</commit_message>
<xml_diff>
--- a/schematics/Full Board Prototype/BOM - Pick & Place etc/Pick & Place.xlsx
+++ b/schematics/Full Board Prototype/BOM - Pick & Place etc/Pick & Place.xlsx
@@ -996,7 +996,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1011,13 +1011,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1361,11 +1360,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,6 +1377,7 @@
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" style="4" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1393,16 +1396,16 @@
       <c r="E1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="8" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1422,16 +1425,16 @@
       <c r="E2" s="5">
         <v>1432109</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="9">
         <v>43.18</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="9">
         <v>76.84</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="9">
         <v>270</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1451,16 +1454,16 @@
       <c r="E3" s="5">
         <v>1432109</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>43.18</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="9">
         <v>40.32</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="9">
         <v>270</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1480,16 +1483,16 @@
       <c r="E4" s="5">
         <v>1432109</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="9">
         <v>43.18</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <v>5.4</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="9">
         <v>270</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1518,7 +1521,7 @@
       <c r="H5" s="9">
         <v>270</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1547,7 +1550,7 @@
       <c r="H6" s="9">
         <v>270</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1576,7 +1579,7 @@
       <c r="H7" s="9">
         <v>270</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1605,7 +1608,7 @@
       <c r="H8" s="9">
         <v>90</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1634,7 +1637,7 @@
       <c r="H9" s="9">
         <v>90</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1663,7 +1666,7 @@
       <c r="H10" s="9">
         <v>90</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1692,7 +1695,7 @@
       <c r="H11" s="9">
         <v>0</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1721,7 +1724,7 @@
       <c r="H12" s="9">
         <v>180</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1750,7 +1753,7 @@
       <c r="H13" s="9">
         <v>0</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1779,7 +1782,7 @@
       <c r="H14" s="9">
         <v>180</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1808,7 +1811,7 @@
       <c r="H15" s="9">
         <v>0</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1837,7 +1840,7 @@
       <c r="H16" s="9">
         <v>180</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1866,7 +1869,7 @@
       <c r="H17" s="9">
         <v>270</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1895,7 +1898,7 @@
       <c r="H18" s="9">
         <v>270</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1924,7 +1927,7 @@
       <c r="H19" s="9">
         <v>270</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1953,7 +1956,7 @@
       <c r="H20" s="9">
         <v>270</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1982,7 +1985,7 @@
       <c r="H21" s="9">
         <v>270</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2011,7 +2014,7 @@
       <c r="H22" s="9">
         <v>270</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2040,7 +2043,7 @@
       <c r="H23" s="9">
         <v>0</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2069,7 +2072,7 @@
       <c r="H24" s="9">
         <v>0</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2098,7 +2101,7 @@
       <c r="H25" s="9">
         <v>0</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2127,7 +2130,7 @@
       <c r="H26" s="9">
         <v>270</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2156,7 +2159,7 @@
       <c r="H27" s="9">
         <v>270</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2185,7 +2188,7 @@
       <c r="H28" s="9">
         <v>270</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2214,7 +2217,7 @@
       <c r="H29" s="9">
         <v>0</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2243,7 +2246,7 @@
       <c r="H30" s="9">
         <v>0</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2272,7 +2275,7 @@
       <c r="H31" s="9">
         <v>0</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2301,7 +2304,7 @@
       <c r="H32" s="9">
         <v>270</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2330,7 +2333,7 @@
       <c r="H33" s="9">
         <v>270</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2359,7 +2362,7 @@
       <c r="H34" s="9">
         <v>270</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2388,7 +2391,7 @@
       <c r="H35" s="9">
         <v>180</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2417,7 +2420,7 @@
       <c r="H36" s="9">
         <v>180</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I36" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2446,7 +2449,7 @@
       <c r="H37" s="9">
         <v>180</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2466,16 +2469,16 @@
       <c r="E38" s="5">
         <v>2362109</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="9">
         <v>35.24</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="9">
         <v>91.44</v>
       </c>
-      <c r="H38" s="10">
+      <c r="H38" s="9">
         <v>270</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2495,16 +2498,16 @@
       <c r="E39" s="5">
         <v>1288204</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="9">
         <v>36.99</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G39" s="9">
         <v>98.11</v>
       </c>
-      <c r="H39" s="10">
+      <c r="H39" s="9">
         <v>90</v>
       </c>
-      <c r="I39" s="14" t="s">
+      <c r="I39" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2524,16 +2527,16 @@
       <c r="E40" s="5">
         <v>2362109</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F40" s="9">
         <v>35.24</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="9">
         <v>54.93</v>
       </c>
-      <c r="H40" s="10">
+      <c r="H40" s="9">
         <v>270</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2553,16 +2556,16 @@
       <c r="E41" s="5">
         <v>1288204</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F41" s="9">
         <v>36.99</v>
       </c>
-      <c r="G41" s="10">
+      <c r="G41" s="9">
         <v>61.6</v>
       </c>
-      <c r="H41" s="10">
+      <c r="H41" s="9">
         <v>90</v>
       </c>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2582,16 +2585,16 @@
       <c r="E42" s="5">
         <v>2362109</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F42" s="9">
         <v>35.24</v>
       </c>
-      <c r="G42" s="10">
+      <c r="G42" s="9">
         <v>20</v>
       </c>
-      <c r="H42" s="10">
+      <c r="H42" s="9">
         <v>270</v>
       </c>
-      <c r="I42" s="14" t="s">
+      <c r="I42" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2611,16 +2614,16 @@
       <c r="E43" s="5">
         <v>1288204</v>
       </c>
-      <c r="F43" s="10">
+      <c r="F43" s="9">
         <v>36.99</v>
       </c>
-      <c r="G43" s="10">
+      <c r="G43" s="9">
         <v>26.67</v>
       </c>
-      <c r="H43" s="10">
+      <c r="H43" s="9">
         <v>90</v>
       </c>
-      <c r="I43" s="14" t="s">
+      <c r="I43" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2640,16 +2643,16 @@
       <c r="E44" s="7">
         <v>1581966</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="9">
         <v>43.7</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="9">
         <v>94.85</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="9">
         <v>90</v>
       </c>
-      <c r="I44" s="14" t="s">
+      <c r="I44" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2669,16 +2672,16 @@
       <c r="E45" s="7">
         <v>1581966</v>
       </c>
-      <c r="F45" s="11">
+      <c r="F45" s="9">
         <v>43.7</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G45" s="9">
         <v>58.34</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="9">
         <v>90</v>
       </c>
-      <c r="I45" s="14" t="s">
+      <c r="I45" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2698,16 +2701,16 @@
       <c r="E46" s="7">
         <v>1581966</v>
       </c>
-      <c r="F46" s="11">
+      <c r="F46" s="9">
         <v>43.7</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="9">
         <v>23.42</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="9">
         <v>90</v>
       </c>
-      <c r="I46" s="14" t="s">
+      <c r="I46" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2727,16 +2730,16 @@
       <c r="E47" s="5">
         <v>2067770</v>
       </c>
-      <c r="F47" s="11">
+      <c r="F47" s="9">
         <v>28.89</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G47" s="9">
         <v>78.58</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="9">
         <v>0</v>
       </c>
-      <c r="I47" s="14" t="s">
+      <c r="I47" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2756,16 +2759,16 @@
       <c r="E48" s="5">
         <v>2067770</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="9">
         <v>28.89</v>
       </c>
-      <c r="G48" s="11">
+      <c r="G48" s="9">
         <v>42.07</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="9">
         <v>0</v>
       </c>
-      <c r="I48" s="14" t="s">
+      <c r="I48" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2785,16 +2788,16 @@
       <c r="E49" s="5">
         <v>2067770</v>
       </c>
-      <c r="F49" s="11">
+      <c r="F49" s="9">
         <v>28.89</v>
       </c>
-      <c r="G49" s="11">
+      <c r="G49" s="9">
         <v>7.14</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="9">
         <v>0</v>
       </c>
-      <c r="I49" s="14" t="s">
+      <c r="I49" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2814,16 +2817,16 @@
       <c r="E50" s="7">
         <v>9732241</v>
       </c>
-      <c r="F50" t="s">
-        <v>159</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I50" s="14" t="s">
+      <c r="F50" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I50" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2843,16 +2846,16 @@
       <c r="E51" s="7">
         <v>9732241</v>
       </c>
-      <c r="F51" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H51" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I51" s="14" t="s">
+      <c r="F51" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I51" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2872,16 +2875,16 @@
       <c r="E52" s="7">
         <v>9732241</v>
       </c>
-      <c r="F52" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G52" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I52" s="14" t="s">
+      <c r="F52" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I52" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2898,16 +2901,16 @@
       <c r="E53" s="5">
         <v>1098038</v>
       </c>
-      <c r="F53" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I53" s="14" t="s">
+      <c r="F53" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I53" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2924,16 +2927,16 @@
       <c r="E54" s="5">
         <v>1098038</v>
       </c>
-      <c r="F54" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G54" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I54" s="14" t="s">
+      <c r="F54" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I54" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2950,16 +2953,16 @@
       <c r="E55" s="5">
         <v>1098038</v>
       </c>
-      <c r="F55" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H55" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I55" s="14" t="s">
+      <c r="F55" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I55" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2976,16 +2979,16 @@
       <c r="E56" s="5">
         <v>1098038</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H56" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I56" s="14" t="s">
+      <c r="F56" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I56" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3002,16 +3005,16 @@
       <c r="E57" s="5">
         <v>1098038</v>
       </c>
-      <c r="F57" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I57" s="14" t="s">
+      <c r="F57" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I57" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3028,16 +3031,16 @@
       <c r="E58" s="5">
         <v>1098038</v>
       </c>
-      <c r="F58" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G58" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H58" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I58" s="14" t="s">
+      <c r="F58" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I58" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3054,16 +3057,16 @@
       <c r="E59" s="5">
         <v>1098038</v>
       </c>
-      <c r="F59" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G59" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H59" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I59" s="14" t="s">
+      <c r="F59" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I59" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3080,16 +3083,16 @@
       <c r="E60" s="5">
         <v>1098038</v>
       </c>
-      <c r="F60" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G60" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I60" s="14" t="s">
+      <c r="F60" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I60" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3106,16 +3109,16 @@
       <c r="E61" s="5">
         <v>1098038</v>
       </c>
-      <c r="F61" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G61" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I61" s="14" t="s">
+      <c r="F61" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I61" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3132,16 +3135,16 @@
       <c r="E62" s="5">
         <v>1098038</v>
       </c>
-      <c r="F62" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I62" s="14" t="s">
+      <c r="F62" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I62" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3158,16 +3161,16 @@
       <c r="E63" s="5">
         <v>1098038</v>
       </c>
-      <c r="F63" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G63" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I63" s="14" t="s">
+      <c r="F63" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I63" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3184,16 +3187,16 @@
       <c r="E64" s="5">
         <v>1098038</v>
       </c>
-      <c r="F64" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G64" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I64" s="14" t="s">
+      <c r="F64" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I64" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3210,16 +3213,16 @@
       <c r="E65" s="5">
         <v>1098038</v>
       </c>
-      <c r="F65" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I65" s="14" t="s">
+      <c r="F65" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I65" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3236,16 +3239,16 @@
       <c r="E66" s="5">
         <v>1098038</v>
       </c>
-      <c r="F66" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H66" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I66" s="14" t="s">
+      <c r="F66" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I66" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3262,16 +3265,16 @@
       <c r="E67" s="5">
         <v>1098038</v>
       </c>
-      <c r="F67" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G67" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H67" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I67" s="14" t="s">
+      <c r="F67" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I67" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3288,16 +3291,16 @@
       <c r="E68" s="5">
         <v>1098038</v>
       </c>
-      <c r="F68" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I68" s="14" t="s">
+      <c r="F68" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I68" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3314,16 +3317,16 @@
       <c r="E69" s="5">
         <v>1098038</v>
       </c>
-      <c r="F69" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G69" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H69" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I69" s="14" t="s">
+      <c r="F69" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I69" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3340,16 +3343,16 @@
       <c r="E70" s="5">
         <v>1098038</v>
       </c>
-      <c r="F70" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G70" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H70" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I70" s="14" t="s">
+      <c r="F70" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I70" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3366,16 +3369,16 @@
       <c r="E71" s="5">
         <v>1098038</v>
       </c>
-      <c r="F71" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H71" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I71" s="14" t="s">
+      <c r="F71" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I71" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3392,16 +3395,16 @@
       <c r="E72" s="5">
         <v>1098038</v>
       </c>
-      <c r="F72" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G72" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H72" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I72" s="14" t="s">
+      <c r="F72" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I72" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3418,16 +3421,16 @@
       <c r="E73" s="5">
         <v>1098038</v>
       </c>
-      <c r="F73" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H73" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I73" s="14" t="s">
+      <c r="F73" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I73" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3444,16 +3447,16 @@
       <c r="E74" s="5">
         <v>1098038</v>
       </c>
-      <c r="F74" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H74" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I74" s="14" t="s">
+      <c r="F74" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I74" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3470,16 +3473,16 @@
       <c r="E75" s="5">
         <v>1098038</v>
       </c>
-      <c r="F75" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G75" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H75" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I75" s="14" t="s">
+      <c r="F75" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I75" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3496,16 +3499,16 @@
       <c r="E76" s="5">
         <v>1098038</v>
       </c>
-      <c r="F76" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H76" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I76" s="14" t="s">
+      <c r="F76" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I76" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3522,16 +3525,16 @@
       <c r="E77" s="5">
         <v>1098038</v>
       </c>
-      <c r="F77" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H77" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I77" s="14" t="s">
+      <c r="F77" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I77" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3548,16 +3551,16 @@
       <c r="E78" s="5">
         <v>1098038</v>
       </c>
-      <c r="F78" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G78" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H78" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I78" s="14" t="s">
+      <c r="F78" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I78" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3574,16 +3577,16 @@
       <c r="E79" s="5">
         <v>1098038</v>
       </c>
-      <c r="F79" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G79" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H79" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I79" s="14" t="s">
+      <c r="F79" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I79" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3600,16 +3603,16 @@
       <c r="E80" s="5">
         <v>1098038</v>
       </c>
-      <c r="F80" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G80" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H80" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I80" s="14" t="s">
+      <c r="F80" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I80" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3626,16 +3629,16 @@
       <c r="E81" s="5">
         <v>1098038</v>
       </c>
-      <c r="F81" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G81" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H81" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I81" s="14" t="s">
+      <c r="F81" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I81" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3652,16 +3655,16 @@
       <c r="E82" s="5">
         <v>1098038</v>
       </c>
-      <c r="F82" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G82" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H82" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I82" s="14" t="s">
+      <c r="F82" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H82" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I82" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3678,16 +3681,16 @@
       <c r="E83" s="5">
         <v>1098038</v>
       </c>
-      <c r="F83" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G83" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H83" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I83" s="14" t="s">
+      <c r="F83" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H83" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I83" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3704,16 +3707,16 @@
       <c r="E84" s="5">
         <v>1098038</v>
       </c>
-      <c r="F84" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G84" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H84" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I84" s="14" t="s">
+      <c r="F84" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I84" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3733,16 +3736,16 @@
       <c r="E85" s="7">
         <v>9732241</v>
       </c>
-      <c r="F85" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G85" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H85" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I85" s="14" t="s">
+      <c r="F85" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H85" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I85" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3759,16 +3762,16 @@
       <c r="E86" s="7">
         <v>9732241</v>
       </c>
-      <c r="F86" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G86" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H86" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I86" s="14" t="s">
+      <c r="F86" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I86" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3788,16 +3791,16 @@
       <c r="E87" s="7">
         <v>1468890</v>
       </c>
-      <c r="F87" s="12">
+      <c r="F87" s="9">
         <v>33.5</v>
       </c>
-      <c r="G87" s="12">
+      <c r="G87" s="9">
         <v>103.19</v>
       </c>
-      <c r="H87" s="12">
+      <c r="H87" s="9">
         <v>180</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3817,16 +3820,16 @@
       <c r="E88" s="7">
         <v>1468890</v>
       </c>
-      <c r="F88" s="12">
+      <c r="F88" s="9">
         <v>33.5</v>
       </c>
-      <c r="G88" s="12">
+      <c r="G88" s="9">
         <v>66.67</v>
       </c>
-      <c r="H88" s="12">
+      <c r="H88" s="9">
         <v>180</v>
       </c>
-      <c r="I88" s="14" t="s">
+      <c r="I88" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3846,16 +3849,16 @@
       <c r="E89" s="7">
         <v>1468890</v>
       </c>
-      <c r="F89" s="12">
+      <c r="F89" s="9">
         <v>33.5</v>
       </c>
-      <c r="G89" s="12">
+      <c r="G89" s="9">
         <v>31.75</v>
       </c>
-      <c r="H89" s="12">
+      <c r="H89" s="9">
         <v>180</v>
       </c>
-      <c r="I89" s="14" t="s">
+      <c r="I89" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3875,16 +3878,16 @@
       <c r="E90" s="7">
         <v>2325323</v>
       </c>
-      <c r="F90" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G90" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H90" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="I90" s="14" t="s">
+      <c r="F90" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I90" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3904,16 +3907,16 @@
       <c r="E91" s="7">
         <v>2325323</v>
       </c>
-      <c r="F91" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G91" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H91" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="I91" s="14" t="s">
+      <c r="F91" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I91" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3933,16 +3936,16 @@
       <c r="E92" s="7">
         <v>2325323</v>
       </c>
-      <c r="F92" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G92" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="H92" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="I92" s="14" t="s">
+      <c r="F92" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I92" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3962,16 +3965,16 @@
       <c r="E93" s="6">
         <v>1838112</v>
       </c>
-      <c r="F93" s="13">
+      <c r="F93" s="9">
         <v>25.08</v>
       </c>
-      <c r="G93" s="13">
+      <c r="G93" s="9">
         <v>89.54</v>
       </c>
-      <c r="H93" s="13">
+      <c r="H93" s="9">
         <v>180</v>
       </c>
-      <c r="I93" s="14" t="s">
+      <c r="I93" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3991,16 +3994,16 @@
       <c r="E94" s="6">
         <v>1837879</v>
       </c>
-      <c r="F94" s="13">
+      <c r="F94" s="9">
         <v>34.93</v>
       </c>
-      <c r="G94" s="13">
+      <c r="G94" s="9">
         <v>97</v>
       </c>
-      <c r="H94" s="13">
+      <c r="H94" s="9">
         <v>270</v>
       </c>
-      <c r="I94" s="14" t="s">
+      <c r="I94" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4020,16 +4023,16 @@
       <c r="E95" s="6">
         <v>1838112</v>
       </c>
-      <c r="F95" s="13">
+      <c r="F95" s="9">
         <v>25.08</v>
       </c>
-      <c r="G95" s="13">
+      <c r="G95" s="9">
         <v>53.02</v>
       </c>
-      <c r="H95" s="13">
+      <c r="H95" s="9">
         <v>180</v>
       </c>
-      <c r="I95" s="14" t="s">
+      <c r="I95" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4049,16 +4052,16 @@
       <c r="E96" s="6">
         <v>1837879</v>
       </c>
-      <c r="F96" s="13">
+      <c r="F96" s="9">
         <v>34.93</v>
       </c>
-      <c r="G96" s="13">
+      <c r="G96" s="9">
         <v>60.48</v>
       </c>
-      <c r="H96" s="13">
+      <c r="H96" s="9">
         <v>270</v>
       </c>
-      <c r="I96" s="14" t="s">
+      <c r="I96" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4078,16 +4081,16 @@
       <c r="E97" s="6">
         <v>1838112</v>
       </c>
-      <c r="F97" s="13">
+      <c r="F97" s="9">
         <v>25.08</v>
       </c>
-      <c r="G97" s="13">
+      <c r="G97" s="9">
         <v>18.100000000000001</v>
       </c>
-      <c r="H97" s="13">
+      <c r="H97" s="9">
         <v>180</v>
       </c>
-      <c r="I97" s="14" t="s">
+      <c r="I97" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4107,16 +4110,16 @@
       <c r="E98" s="6">
         <v>1837879</v>
       </c>
-      <c r="F98" s="13">
+      <c r="F98" s="9">
         <v>34.93</v>
       </c>
-      <c r="G98" s="13">
+      <c r="G98" s="9">
         <v>25.56</v>
       </c>
-      <c r="H98" s="13">
+      <c r="H98" s="9">
         <v>270</v>
       </c>
-      <c r="I98" s="14" t="s">
+      <c r="I98" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4136,16 +4139,16 @@
       <c r="E99" s="6">
         <v>2131042</v>
       </c>
-      <c r="F99" s="13">
+      <c r="F99" s="9">
         <v>40.32</v>
       </c>
-      <c r="G99" s="13">
+      <c r="G99" s="9">
         <v>76.84</v>
       </c>
-      <c r="H99" s="13">
+      <c r="H99" s="9">
         <v>270</v>
       </c>
-      <c r="I99" s="14" t="s">
+      <c r="I99" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4165,16 +4168,16 @@
       <c r="E100" s="6">
         <v>2131042</v>
       </c>
-      <c r="F100" s="13">
+      <c r="F100" s="9">
         <v>40.32</v>
       </c>
-      <c r="G100" s="13">
+      <c r="G100" s="9">
         <v>40.32</v>
       </c>
-      <c r="H100" s="13">
+      <c r="H100" s="9">
         <v>270</v>
       </c>
-      <c r="I100" s="14" t="s">
+      <c r="I100" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4194,16 +4197,16 @@
       <c r="E101" s="6">
         <v>2131042</v>
       </c>
-      <c r="F101" s="13">
+      <c r="F101" s="9">
         <v>40.32</v>
       </c>
-      <c r="G101" s="13">
+      <c r="G101" s="9">
         <v>5.4</v>
       </c>
-      <c r="H101" s="13">
+      <c r="H101" s="9">
         <v>270</v>
       </c>
-      <c r="I101" s="14" t="s">
+      <c r="I101" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4223,16 +4226,16 @@
       <c r="E102" s="7">
         <v>2068091</v>
       </c>
-      <c r="F102" s="13">
+      <c r="F102" s="9">
         <v>28.26</v>
       </c>
-      <c r="G102" s="13">
+      <c r="G102" s="9">
         <v>94.77</v>
       </c>
-      <c r="H102" s="13">
+      <c r="H102" s="9">
         <v>270</v>
       </c>
-      <c r="I102" s="14" t="s">
+      <c r="I102" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4252,16 +4255,16 @@
       <c r="E103" s="7">
         <v>2068091</v>
       </c>
-      <c r="F103" s="13">
+      <c r="F103" s="9">
         <v>28.26</v>
       </c>
-      <c r="G103" s="13">
+      <c r="G103" s="9">
         <v>58.26</v>
       </c>
-      <c r="H103" s="13">
+      <c r="H103" s="9">
         <v>270</v>
       </c>
-      <c r="I103" s="14" t="s">
+      <c r="I103" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4281,16 +4284,16 @@
       <c r="E104" s="7">
         <v>2068091</v>
       </c>
-      <c r="F104" s="13">
+      <c r="F104" s="9">
         <v>28.26</v>
       </c>
-      <c r="G104" s="13">
+      <c r="G104" s="9">
         <v>23.34</v>
       </c>
-      <c r="H104" s="13">
+      <c r="H104" s="9">
         <v>270</v>
       </c>
-      <c r="I104" s="14" t="s">
+      <c r="I104" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4310,16 +4313,16 @@
       <c r="E105" s="7">
         <v>9604367</v>
       </c>
-      <c r="F105" s="14">
+      <c r="F105" s="9">
         <v>9.2100000000000009</v>
       </c>
-      <c r="G105" s="14">
+      <c r="G105" s="9">
         <v>68.58</v>
       </c>
-      <c r="H105" s="14">
+      <c r="H105" s="9">
         <v>0</v>
       </c>
-      <c r="I105" s="14" t="s">
+      <c r="I105" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4339,16 +4342,16 @@
       <c r="E106" s="6">
         <v>8391289</v>
       </c>
-      <c r="F106" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G106" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H106" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I106" t="s">
+      <c r="F106" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H106" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I106" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4368,16 +4371,16 @@
       <c r="E107" s="6">
         <v>2294307</v>
       </c>
-      <c r="F107" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G107" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H107" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I107" t="s">
+      <c r="F107" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H107" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I107" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4397,16 +4400,16 @@
       <c r="E108" s="6">
         <v>1084697</v>
       </c>
-      <c r="F108" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G108" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H108" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I108" t="s">
+      <c r="F108" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H108" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I108" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4448,6 +4451,6 @@
     <hyperlink ref="E70:E84" r:id="rId25" tooltip="1098038" display="http://uk.farnell.com/fci/76341-308lf/socket-1row-8way/dp/1098038"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId26"/>
+  <pageSetup paperSize="9" scale="79" fitToHeight="0" orientation="landscape" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>